<commit_message>
Adding accessory documents for project 1
</commit_message>
<xml_diff>
--- a/project1Skeleton/project1_skeleton/part2aData.xlsx
+++ b/project1Skeleton/project1_skeleton/part2aData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2aOutput" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>NumDocs</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>MaxWaitl_l1</t>
+  </si>
+  <si>
+    <t>busyness</t>
   </si>
 </sst>
 </file>
@@ -1231,11 +1234,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76169216"/>
-        <c:axId val="75805824"/>
+        <c:axId val="87982464"/>
+        <c:axId val="87984000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76169216"/>
+        <c:axId val="87982464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,12 +1248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75805824"/>
+        <c:crossAx val="87984000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75805824"/>
+        <c:axId val="87984000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,7 +1264,244 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76169216"/>
+        <c:crossAx val="87982464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>busyness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>99.976045035333499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.916618220450005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.808869347400105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.688652717683894</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.512517927013405</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.303249470361294</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.090087456004198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98.881502065243197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>98.408219110476097</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97.697305116556095</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96.663906518200093</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>94.529617969399098</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.897343567511996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.922332142554595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80.263699686975798</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75.849370656717298</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>71.328741125856297</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>67.423085526190704</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>63.765689098418399</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60.589499758494703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="77047680"/>
+        <c:axId val="77046144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="77047680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77046144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="77046144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77047680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1301,6 +1541,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1607,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" activeCellId="2" sqref="C7 A1:A1048576 J1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,12 +2953,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>99.976045035333499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>99.916618220450005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>99.808869347400105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>99.688652717683894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>99.512517927013405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>99.303249470361294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>99.090087456004198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>98.881502065243197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>98.408219110476097</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>97.697305116556095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>96.663906518200093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>94.529617969399098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>90.897343567511996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>85.922332142554595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>80.263699686975798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>75.849370656717298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>71.328741125856297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>67.423085526190704</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>63.765689098418399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>60.589499758494703</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>